<commit_message>
added mapping on service level between TM and OJP
</commit_message>
<xml_diff>
--- a/docs/transmodel_ojp_mapping/Mapping_OJP_TRANSMODEL_V3.0.xlsx
+++ b/docs/transmodel_ojp_mapping/Mapping_OJP_TRANSMODEL_V3.0.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ue71603\MG_Daten\github\OJP4\docs\transmodel_ojp_mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C701F349-60FC-4ECE-B7BB-4D105B3E28FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF487ED-2D63-4E6A-B7E3-3D6C89B00CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-54285" yWindow="9090" windowWidth="21600" windowHeight="12495" tabRatio="469" activeTab="2" xr2:uid="{92A06D46-43C6-42FE-B5E0-5A99A190FF7F}"/>
+    <workbookView xWindow="67080" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="469" xr2:uid="{92A06D46-43C6-42FE-B5E0-5A99A190FF7F}"/>
   </bookViews>
   <sheets>
-    <sheet name="OJPTrip" sheetId="1" r:id="rId1"/>
-    <sheet name="OJPPlaceInformation" sheetId="3" r:id="rId2"/>
-    <sheet name="OJPStopEvent" sheetId="2" r:id="rId3"/>
-    <sheet name="OJPExchangePoint" sheetId="4" r:id="rId4"/>
-    <sheet name="OJPMultiPointTrip" sheetId="5" r:id="rId5"/>
-    <sheet name="OJPFare" sheetId="6" r:id="rId6"/>
-    <sheet name="OJPTripInformation" sheetId="7" r:id="rId7"/>
-    <sheet name="OJPAvailability" sheetId="8" r:id="rId8"/>
+    <sheet name="Mapping_Services_QUERY_MODEL" sheetId="9" r:id="rId1"/>
+    <sheet name="OJPTrip" sheetId="1" r:id="rId2"/>
+    <sheet name="OJPPlaceInformation" sheetId="3" r:id="rId3"/>
+    <sheet name="OJPStopEvent" sheetId="2" r:id="rId4"/>
+    <sheet name="OJPExchangePoint" sheetId="4" r:id="rId5"/>
+    <sheet name="OJPMultiPointTrip" sheetId="5" r:id="rId6"/>
+    <sheet name="OJPFare" sheetId="6" r:id="rId7"/>
+    <sheet name="OJPTripInformation" sheetId="7" r:id="rId8"/>
+    <sheet name="OJPAvailability" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2670" uniqueCount="1021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2719" uniqueCount="1049">
   <si>
     <t>column H and I are the important part, H should describe, what happens</t>
   </si>
@@ -3111,6 +3112,91 @@
   </si>
   <si>
     <t>OJPAvailabilityResponse</t>
+  </si>
+  <si>
+    <t>OJP</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>SCHEDULE REQUEST</t>
+  </si>
+  <si>
+    <t>EXCHANGE POINTS REQUST</t>
+  </si>
+  <si>
+    <t>SITUATION REQUEST</t>
+  </si>
+  <si>
+    <t>SERVICE JOURNEY REQUEST</t>
+  </si>
+  <si>
+    <t>STOP FARE REQUEST</t>
+  </si>
+  <si>
+    <t>FARE PRODUCT REQUST</t>
+  </si>
+  <si>
+    <t>TRIP FARE REQUEST</t>
+  </si>
+  <si>
+    <t>OJPTripRequest
+OJPMultipointTripRequest</t>
+  </si>
+  <si>
+    <t>OJPStopEventRequest</t>
+  </si>
+  <si>
+    <t>OJPTripInformationRequest</t>
+  </si>
+  <si>
+    <t>Not implemented in OJP</t>
+  </si>
+  <si>
+    <t>Situations are delivered in the results of other requests (e.g. OJPLocationInformationRequest, OJPStopEventRequest, OJPTripRequest)</t>
+  </si>
+  <si>
+    <t>OJPLocationInformationRequest</t>
+  </si>
+  <si>
+    <t>All within OJPFareRequest</t>
+  </si>
+  <si>
+    <t>Asks for the availability of a VEHICLE, SINGLE JOURNEY</t>
+  </si>
+  <si>
+    <t>OJPExchangePointsRequest</t>
+  </si>
+  <si>
+    <t>OJPLineInformationRequest</t>
+  </si>
+  <si>
+    <t>OJPStatusRequest</t>
+  </si>
+  <si>
+    <t>Informs about the trip planner</t>
+  </si>
+  <si>
+    <t>OJPTripChangeRequest</t>
+  </si>
+  <si>
+    <t>OJPTripRefineRequest</t>
+  </si>
+  <si>
+    <t>Provides details about a LINE</t>
+  </si>
+  <si>
+    <t>Allows to update a TRIP REQUEST from an already made TRIP RESULT</t>
+  </si>
+  <si>
+    <t>Adds more details to given TRIP RESULTS</t>
+  </si>
+  <si>
+    <t>Mapping of the abstract Transmodel services to OJP</t>
+  </si>
+  <si>
+    <t>Transmodel</t>
   </si>
 </sst>
 </file>
@@ -3404,7 +3490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3616,19 +3702,19 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3664,6 +3750,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -4175,11 +4262,213 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AAB1CDC-A2F2-4A06-BB2E-638A1C365426}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="23.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.86328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="89" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="12" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E8571E6-8D43-44CC-B9D0-687AC8D4191F}">
   <dimension ref="A1:Q208"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="11" topLeftCell="G90" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="11" topLeftCell="G54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="M106" sqref="A1:XFD1048576"/>
@@ -4249,15 +4538,15 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
-      <c r="K7" s="74" t="s">
+      <c r="K7" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="74"/>
+      <c r="L7" s="77"/>
+      <c r="M7" s="77"/>
+      <c r="N7" s="77"/>
+      <c r="O7" s="77"/>
+      <c r="P7" s="77"/>
+      <c r="Q7" s="77"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" s="78" t="s">
@@ -4281,34 +4570,34 @@
       <c r="G8" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="76" t="s">
+      <c r="I8" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="75" t="s">
+      <c r="J8" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="75" t="s">
+      <c r="K8" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="75" t="s">
+      <c r="L8" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="75" t="s">
+      <c r="M8" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="75" t="s">
+      <c r="N8" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="73" t="s">
+      <c r="O8" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="73" t="s">
+      <c r="P8" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="73" t="s">
+      <c r="Q8" s="74" t="s">
         <v>24</v>
       </c>
     </row>
@@ -4324,18 +4613,18 @@
       </c>
       <c r="F9" s="80"/>
       <c r="G9" s="78"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="73"/>
-      <c r="P9" s="73" t="s">
+      <c r="H9" s="73"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="73"/>
+      <c r="N9" s="73"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="Q9" s="73"/>
+      <c r="Q9" s="74"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" s="78"/>
@@ -4347,16 +4636,16 @@
       </c>
       <c r="F10" s="80"/>
       <c r="G10" s="78"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="75"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="75"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="73"/>
+      <c r="H10" s="73"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="73"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="73"/>
+      <c r="N10" s="73"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
     </row>
     <row r="11" spans="1:17" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="78"/>
@@ -4368,16 +4657,16 @@
       </c>
       <c r="F11" s="80"/>
       <c r="G11" s="78"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="75"/>
-      <c r="N11" s="75"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="73"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
+      <c r="M11" s="73"/>
+      <c r="N11" s="73"/>
+      <c r="O11" s="74"/>
+      <c r="P11" s="74"/>
+      <c r="Q11" s="74"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B12" s="1" t="s">
@@ -7423,6 +7712,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="Q8:Q11"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="J8:J11"/>
+    <mergeCell ref="K8:K11"/>
+    <mergeCell ref="L8:L11"/>
+    <mergeCell ref="N8:N11"/>
+    <mergeCell ref="O8:O11"/>
+    <mergeCell ref="M8:M11"/>
     <mergeCell ref="H8:H11"/>
     <mergeCell ref="P8:P11"/>
     <mergeCell ref="I8:I11"/>
@@ -7431,21 +7728,13 @@
     <mergeCell ref="C8:C11"/>
     <mergeCell ref="F8:F11"/>
     <mergeCell ref="G8:G11"/>
-    <mergeCell ref="Q8:Q11"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="J8:J11"/>
-    <mergeCell ref="K8:K11"/>
-    <mergeCell ref="L8:L11"/>
-    <mergeCell ref="N8:N11"/>
-    <mergeCell ref="O8:O11"/>
-    <mergeCell ref="M8:M11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67F5C9FB-EB55-4D3D-AE2C-4A2AE611540E}">
   <dimension ref="A1:Q137"/>
   <sheetViews>
@@ -7520,15 +7809,15 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
-      <c r="K7" s="74" t="s">
+      <c r="K7" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="74"/>
+      <c r="L7" s="77"/>
+      <c r="M7" s="77"/>
+      <c r="N7" s="77"/>
+      <c r="O7" s="77"/>
+      <c r="P7" s="77"/>
+      <c r="Q7" s="77"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" s="78" t="s">
@@ -7552,34 +7841,34 @@
       <c r="G8" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="76" t="s">
+      <c r="I8" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="75" t="s">
+      <c r="J8" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="75" t="s">
+      <c r="K8" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="75" t="s">
+      <c r="L8" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="75" t="s">
+      <c r="M8" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="75" t="s">
+      <c r="N8" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="73" t="s">
+      <c r="O8" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="73" t="s">
+      <c r="P8" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="73" t="s">
+      <c r="Q8" s="74" t="s">
         <v>24</v>
       </c>
     </row>
@@ -7595,18 +7884,18 @@
       </c>
       <c r="F9" s="80"/>
       <c r="G9" s="78"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="73"/>
-      <c r="P9" s="73" t="s">
+      <c r="H9" s="73"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="73"/>
+      <c r="N9" s="73"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="Q9" s="73"/>
+      <c r="Q9" s="74"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" s="78"/>
@@ -7618,16 +7907,16 @@
       </c>
       <c r="F10" s="80"/>
       <c r="G10" s="78"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="75"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="75"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="73"/>
+      <c r="H10" s="73"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="73"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="73"/>
+      <c r="N10" s="73"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
     </row>
     <row r="11" spans="1:17" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="78"/>
@@ -7639,16 +7928,16 @@
       </c>
       <c r="F11" s="80"/>
       <c r="G11" s="78"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="75"/>
-      <c r="N11" s="75"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="73"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
+      <c r="M11" s="73"/>
+      <c r="N11" s="73"/>
+      <c r="O11" s="74"/>
+      <c r="P11" s="74"/>
+      <c r="Q11" s="74"/>
     </row>
     <row r="12" spans="1:17" ht="57" x14ac:dyDescent="0.45">
       <c r="B12" s="12" t="s">
@@ -9621,11 +9910,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{263B0D09-B6E7-4C7C-ACBE-4F7EEED01E54}">
   <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="11" topLeftCell="I65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -12027,7 +12316,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D88EFA50-F472-477D-861C-0C84615FC860}">
   <dimension ref="A1:Q94"/>
   <sheetViews>
@@ -12102,15 +12391,15 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
-      <c r="K7" s="74" t="s">
+      <c r="K7" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="74"/>
+      <c r="L7" s="77"/>
+      <c r="M7" s="77"/>
+      <c r="N7" s="77"/>
+      <c r="O7" s="77"/>
+      <c r="P7" s="77"/>
+      <c r="Q7" s="77"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" s="78" t="s">
@@ -12134,34 +12423,34 @@
       <c r="G8" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="76" t="s">
+      <c r="I8" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="75" t="s">
+      <c r="J8" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="75" t="s">
+      <c r="K8" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="75" t="s">
+      <c r="L8" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="75" t="s">
+      <c r="M8" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="75" t="s">
+      <c r="N8" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="73" t="s">
+      <c r="O8" s="74" t="s">
         <v>898</v>
       </c>
-      <c r="P8" s="73" t="s">
+      <c r="P8" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="73" t="s">
+      <c r="Q8" s="74" t="s">
         <v>24</v>
       </c>
     </row>
@@ -12177,18 +12466,18 @@
       </c>
       <c r="F9" s="80"/>
       <c r="G9" s="78"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="73"/>
-      <c r="P9" s="73" t="s">
+      <c r="H9" s="73"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="73"/>
+      <c r="N9" s="73"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="Q9" s="73"/>
+      <c r="Q9" s="74"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" s="78"/>
@@ -12200,16 +12489,16 @@
       </c>
       <c r="F10" s="80"/>
       <c r="G10" s="78"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="75"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="75"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="73"/>
+      <c r="H10" s="73"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="73"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="73"/>
+      <c r="N10" s="73"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
     </row>
     <row r="11" spans="1:17" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="78"/>
@@ -12221,16 +12510,16 @@
       </c>
       <c r="F11" s="80"/>
       <c r="G11" s="78"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="75"/>
-      <c r="N11" s="75"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="73"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
+      <c r="M11" s="73"/>
+      <c r="N11" s="73"/>
+      <c r="O11" s="74"/>
+      <c r="P11" s="74"/>
+      <c r="Q11" s="74"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B12" s="12" t="s">
@@ -13592,7 +13881,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E226BA5-A209-4D27-B7B0-834B796D9DCE}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
@@ -13667,15 +13956,15 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
-      <c r="K7" s="74" t="s">
+      <c r="K7" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="74"/>
+      <c r="L7" s="77"/>
+      <c r="M7" s="77"/>
+      <c r="N7" s="77"/>
+      <c r="O7" s="77"/>
+      <c r="P7" s="77"/>
+      <c r="Q7" s="77"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" s="78" t="s">
@@ -13699,34 +13988,34 @@
       <c r="G8" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="76" t="s">
+      <c r="I8" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="75" t="s">
+      <c r="J8" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="75" t="s">
+      <c r="K8" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="75" t="s">
+      <c r="L8" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="75" t="s">
+      <c r="M8" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="75" t="s">
+      <c r="N8" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="73" t="s">
+      <c r="O8" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="73" t="s">
+      <c r="P8" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="73" t="s">
+      <c r="Q8" s="74" t="s">
         <v>24</v>
       </c>
     </row>
@@ -13742,18 +14031,18 @@
       </c>
       <c r="F9" s="80"/>
       <c r="G9" s="78"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="73"/>
-      <c r="P9" s="73" t="s">
+      <c r="H9" s="73"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="73"/>
+      <c r="N9" s="73"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="Q9" s="73"/>
+      <c r="Q9" s="74"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" s="78"/>
@@ -13765,16 +14054,16 @@
       </c>
       <c r="F10" s="80"/>
       <c r="G10" s="78"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="75"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="75"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="73"/>
+      <c r="H10" s="73"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="73"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="73"/>
+      <c r="N10" s="73"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
     </row>
     <row r="11" spans="1:17" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="78"/>
@@ -13786,16 +14075,16 @@
       </c>
       <c r="F11" s="80"/>
       <c r="G11" s="78"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="75"/>
-      <c r="N11" s="75"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="73"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
+      <c r="M11" s="73"/>
+      <c r="N11" s="73"/>
+      <c r="O11" s="74"/>
+      <c r="P11" s="74"/>
+      <c r="Q11" s="74"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B12" s="12" t="s">
@@ -13891,7 +14180,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB81E20B-984F-4AFA-941D-66CD7064B644}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
@@ -13966,15 +14255,15 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
-      <c r="K7" s="74" t="s">
+      <c r="K7" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="74"/>
+      <c r="L7" s="77"/>
+      <c r="M7" s="77"/>
+      <c r="N7" s="77"/>
+      <c r="O7" s="77"/>
+      <c r="P7" s="77"/>
+      <c r="Q7" s="77"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" s="78" t="s">
@@ -13998,34 +14287,34 @@
       <c r="G8" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="76" t="s">
+      <c r="I8" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="75" t="s">
+      <c r="J8" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="75" t="s">
+      <c r="K8" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="75" t="s">
+      <c r="L8" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="75" t="s">
+      <c r="M8" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="75" t="s">
+      <c r="N8" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="73" t="s">
+      <c r="O8" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="73" t="s">
+      <c r="P8" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="73" t="s">
+      <c r="Q8" s="74" t="s">
         <v>24</v>
       </c>
     </row>
@@ -14041,18 +14330,18 @@
       </c>
       <c r="F9" s="80"/>
       <c r="G9" s="78"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="73"/>
-      <c r="P9" s="73" t="s">
+      <c r="H9" s="73"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="73"/>
+      <c r="N9" s="73"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="Q9" s="73"/>
+      <c r="Q9" s="74"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" s="78"/>
@@ -14064,16 +14353,16 @@
       </c>
       <c r="F10" s="80"/>
       <c r="G10" s="78"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="75"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="75"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="73"/>
+      <c r="H10" s="73"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="73"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="73"/>
+      <c r="N10" s="73"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
     </row>
     <row r="11" spans="1:17" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="78"/>
@@ -14085,16 +14374,16 @@
       </c>
       <c r="F11" s="80"/>
       <c r="G11" s="78"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="75"/>
-      <c r="N11" s="75"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="73"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
+      <c r="M11" s="73"/>
+      <c r="N11" s="73"/>
+      <c r="O11" s="74"/>
+      <c r="P11" s="74"/>
+      <c r="Q11" s="74"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B12" s="12" t="s">
@@ -14141,7 +14430,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB730EB-B5B4-4F44-BC03-FF58454E5B15}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
@@ -14216,15 +14505,15 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
-      <c r="K7" s="74" t="s">
+      <c r="K7" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="74"/>
+      <c r="L7" s="77"/>
+      <c r="M7" s="77"/>
+      <c r="N7" s="77"/>
+      <c r="O7" s="77"/>
+      <c r="P7" s="77"/>
+      <c r="Q7" s="77"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" s="78" t="s">
@@ -14248,34 +14537,34 @@
       <c r="G8" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="76" t="s">
+      <c r="I8" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="75" t="s">
+      <c r="J8" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="75" t="s">
+      <c r="K8" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="75" t="s">
+      <c r="L8" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="75" t="s">
+      <c r="M8" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="75" t="s">
+      <c r="N8" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="73" t="s">
+      <c r="O8" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="73" t="s">
+      <c r="P8" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="73" t="s">
+      <c r="Q8" s="74" t="s">
         <v>24</v>
       </c>
     </row>
@@ -14291,18 +14580,18 @@
       </c>
       <c r="F9" s="80"/>
       <c r="G9" s="78"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="73"/>
-      <c r="P9" s="73" t="s">
+      <c r="H9" s="73"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="73"/>
+      <c r="N9" s="73"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="Q9" s="73"/>
+      <c r="Q9" s="74"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" s="78"/>
@@ -14314,16 +14603,16 @@
       </c>
       <c r="F10" s="80"/>
       <c r="G10" s="78"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="75"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="75"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="73"/>
+      <c r="H10" s="73"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="73"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="73"/>
+      <c r="N10" s="73"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
     </row>
     <row r="11" spans="1:17" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="78"/>
@@ -14335,16 +14624,16 @@
       </c>
       <c r="F11" s="80"/>
       <c r="G11" s="78"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="75"/>
-      <c r="N11" s="75"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="73"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
+      <c r="M11" s="73"/>
+      <c r="N11" s="73"/>
+      <c r="O11" s="74"/>
+      <c r="P11" s="74"/>
+      <c r="Q11" s="74"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B12" s="12" t="s">
@@ -14391,7 +14680,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1A5EACF-ADC6-4FEB-8695-B5A0F0F2CF40}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
@@ -14466,15 +14755,15 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
-      <c r="K7" s="74" t="s">
+      <c r="K7" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="74"/>
+      <c r="L7" s="77"/>
+      <c r="M7" s="77"/>
+      <c r="N7" s="77"/>
+      <c r="O7" s="77"/>
+      <c r="P7" s="77"/>
+      <c r="Q7" s="77"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" s="78" t="s">
@@ -14498,34 +14787,34 @@
       <c r="G8" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="76" t="s">
+      <c r="I8" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="75" t="s">
+      <c r="J8" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="75" t="s">
+      <c r="K8" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="75" t="s">
+      <c r="L8" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="75" t="s">
+      <c r="M8" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="75" t="s">
+      <c r="N8" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="73" t="s">
+      <c r="O8" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="73" t="s">
+      <c r="P8" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="73" t="s">
+      <c r="Q8" s="74" t="s">
         <v>24</v>
       </c>
     </row>
@@ -14541,18 +14830,18 @@
       </c>
       <c r="F9" s="80"/>
       <c r="G9" s="78"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="73"/>
-      <c r="P9" s="73" t="s">
+      <c r="H9" s="73"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="73"/>
+      <c r="M9" s="73"/>
+      <c r="N9" s="73"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="Q9" s="73"/>
+      <c r="Q9" s="74"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" s="78"/>
@@ -14564,16 +14853,16 @@
       </c>
       <c r="F10" s="80"/>
       <c r="G10" s="78"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="75"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="75"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="73"/>
+      <c r="H10" s="73"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="73"/>
+      <c r="K10" s="73"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="73"/>
+      <c r="N10" s="73"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
     </row>
     <row r="11" spans="1:17" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="78"/>
@@ -14585,16 +14874,16 @@
       </c>
       <c r="F11" s="80"/>
       <c r="G11" s="78"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="75"/>
-      <c r="N11" s="75"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="73"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
+      <c r="M11" s="73"/>
+      <c r="N11" s="73"/>
+      <c r="O11" s="74"/>
+      <c r="P11" s="74"/>
+      <c r="Q11" s="74"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B12" s="12" t="s">
@@ -14642,14 +14931,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="5cb10dfb-6994-4939-a684-a8afac073853" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6d31159e-acee-463f-b982-d8404a695cd9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14844,27 +15131,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="5cb10dfb-6994-4939-a684-a8afac073853" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6d31159e-acee-463f-b982-d8404a695cd9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{653B82CE-EE8E-41C3-B660-792AB41AF78C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{238E1B12-F9AE-473C-9D3A-C66B2E1D37A4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5cb10dfb-6994-4939-a684-a8afac073853"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="6d31159e-acee-463f-b982-d8404a695cd9"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -14889,9 +15169,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{238E1B12-F9AE-473C-9D3A-C66B2E1D37A4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{653B82CE-EE8E-41C3-B660-792AB41AF78C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5cb10dfb-6994-4939-a684-a8afac073853"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="6d31159e-acee-463f-b982-d8404a695cd9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update mapping after discussion
</commit_message>
<xml_diff>
--- a/docs/transmodel_ojp_mapping/Mapping_OJP_TRANSMODEL_V3.0.xlsx
+++ b/docs/transmodel_ojp_mapping/Mapping_OJP_TRANSMODEL_V3.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ue71603\MG_Daten\github\OJP4\docs\transmodel_ojp_mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF487ED-2D63-4E6A-B7E3-3D6C89B00CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA58C3F1-8757-435B-8C0D-576DBDB3AE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67080" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="469" xr2:uid="{92A06D46-43C6-42FE-B5E0-5A99A190FF7F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" tabRatio="469" xr2:uid="{92A06D46-43C6-42FE-B5E0-5A99A190FF7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping_Services_QUERY_MODEL" sheetId="9" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="OJPAvailability" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2719" uniqueCount="1049">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2716" uniqueCount="1048">
   <si>
     <t>column H and I are the important part, H should describe, what happens</t>
   </si>
@@ -3120,9 +3121,6 @@
     <t>Remarks</t>
   </si>
   <si>
-    <t>SCHEDULE REQUEST</t>
-  </si>
-  <si>
     <t>EXCHANGE POINTS REQUST</t>
   </si>
   <si>
@@ -3151,9 +3149,6 @@
     <t>OJPTripInformationRequest</t>
   </si>
   <si>
-    <t>Not implemented in OJP</t>
-  </si>
-  <si>
     <t>Situations are delivered in the results of other requests (e.g. OJPLocationInformationRequest, OJPStopEventRequest, OJPTripRequest)</t>
   </si>
   <si>
@@ -3169,9 +3164,6 @@
     <t>OJPExchangePointsRequest</t>
   </si>
   <si>
-    <t>OJPLineInformationRequest</t>
-  </si>
-  <si>
     <t>OJPStatusRequest</t>
   </si>
   <si>
@@ -3184,9 +3176,6 @@
     <t>OJPTripRefineRequest</t>
   </si>
   <si>
-    <t>Provides details about a LINE</t>
-  </si>
-  <si>
     <t>Allows to update a TRIP REQUEST from an already made TRIP RESULT</t>
   </si>
   <si>
@@ -3197,6 +3186,15 @@
   </si>
   <si>
     <t>Transmodel</t>
+  </si>
+  <si>
+    <t>(SCHEDULE REQUEST)</t>
+  </si>
+  <si>
+    <t>(OJPLineInformationRequest)</t>
+  </si>
+  <si>
+    <t>With OJPLineInformationRequest some information about a LINE is provided. This is a part of SCHEDULE REQUEST.</t>
   </si>
 </sst>
 </file>
@@ -3702,19 +3700,20 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3750,7 +3749,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -4263,10 +4261,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AAB1CDC-A2F2-4A06-BB2E-638A1C365426}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C18"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4277,13 +4275,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="89" t="s">
-        <v>1047</v>
+      <c r="A1" s="73" t="s">
+        <v>1043</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
-        <v>1048</v>
+        <v>1044</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>1021</v>
@@ -4297,29 +4295,29 @@
         <v>391</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>1023</v>
+        <v>1045</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>1046</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1033</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="C6" s="24" t="s">
         <v>32</v>
@@ -4327,13 +4325,13 @@
     </row>
     <row r="7" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
@@ -4341,7 +4339,7 @@
         <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="C8" s="24" t="s">
         <v>32</v>
@@ -4352,7 +4350,7 @@
         <v>606</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="C9" s="24" t="s">
         <v>32</v>
@@ -4360,10 +4358,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="C10" s="24" t="s">
         <v>32</v>
@@ -4371,35 +4369,35 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>1014</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1014</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>1014</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
@@ -4410,7 +4408,7 @@
         <v>1019</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
@@ -4418,43 +4416,32 @@
         <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1044</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>1041</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>1042</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>1043</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>1046</v>
       </c>
     </row>
   </sheetData>
@@ -4538,24 +4525,24 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
-      <c r="K7" s="77" t="s">
+      <c r="K7" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="77"/>
-      <c r="M7" s="77"/>
-      <c r="N7" s="77"/>
-      <c r="O7" s="77"/>
-      <c r="P7" s="77"/>
-      <c r="Q7" s="77"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
+      <c r="Q7" s="75"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -4564,31 +4551,31 @@
       <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="80" t="s">
+      <c r="F8" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="78" t="s">
+      <c r="G8" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="73" t="s">
+      <c r="H8" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="75" t="s">
+      <c r="I8" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="73" t="s">
+      <c r="J8" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="73" t="s">
+      <c r="K8" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="73" t="s">
+      <c r="L8" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="73" t="s">
+      <c r="M8" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="73" t="s">
+      <c r="N8" s="76" t="s">
         <v>21</v>
       </c>
       <c r="O8" s="74" t="s">
@@ -4602,24 +4589,24 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A9" s="78"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="79"/>
+      <c r="A9" s="79"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="80"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="73"/>
-      <c r="M9" s="73"/>
-      <c r="N9" s="73"/>
+      <c r="F9" s="81"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
       <c r="O9" s="74"/>
       <c r="P9" s="74" t="s">
         <v>27</v>
@@ -4627,43 +4614,43 @@
       <c r="Q9" s="74"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A10" s="78"/>
-      <c r="B10" s="78"/>
-      <c r="C10" s="79"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="5"/>
       <c r="E10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="80"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
-      <c r="N10" s="73"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
       <c r="O10" s="74"/>
       <c r="P10" s="74"/>
       <c r="Q10" s="74"/>
     </row>
     <row r="11" spans="1:17" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="78"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="79"/>
+      <c r="A11" s="79"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="6"/>
       <c r="E11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="80"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="77"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
-      <c r="M11" s="73"/>
-      <c r="N11" s="73"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="76"/>
       <c r="O11" s="74"/>
       <c r="P11" s="74"/>
       <c r="Q11" s="74"/>
@@ -7712,6 +7699,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="H8:H11"/>
+    <mergeCell ref="P8:P11"/>
+    <mergeCell ref="I8:I11"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="F8:F11"/>
+    <mergeCell ref="G8:G11"/>
     <mergeCell ref="Q8:Q11"/>
     <mergeCell ref="K7:Q7"/>
     <mergeCell ref="J8:J11"/>
@@ -7720,14 +7715,6 @@
     <mergeCell ref="N8:N11"/>
     <mergeCell ref="O8:O11"/>
     <mergeCell ref="M8:M11"/>
-    <mergeCell ref="H8:H11"/>
-    <mergeCell ref="P8:P11"/>
-    <mergeCell ref="I8:I11"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="F8:F11"/>
-    <mergeCell ref="G8:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -7809,24 +7796,24 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
-      <c r="K7" s="77" t="s">
+      <c r="K7" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="77"/>
-      <c r="M7" s="77"/>
-      <c r="N7" s="77"/>
-      <c r="O7" s="77"/>
-      <c r="P7" s="77"/>
-      <c r="Q7" s="77"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
+      <c r="Q7" s="75"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -7835,31 +7822,31 @@
       <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="80" t="s">
+      <c r="F8" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="78" t="s">
+      <c r="G8" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="73" t="s">
+      <c r="H8" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="75" t="s">
+      <c r="I8" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="73" t="s">
+      <c r="J8" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="73" t="s">
+      <c r="K8" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="73" t="s">
+      <c r="L8" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="73" t="s">
+      <c r="M8" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="73" t="s">
+      <c r="N8" s="76" t="s">
         <v>21</v>
       </c>
       <c r="O8" s="74" t="s">
@@ -7873,24 +7860,24 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A9" s="78"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="79"/>
+      <c r="A9" s="79"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="80"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="73"/>
-      <c r="M9" s="73"/>
-      <c r="N9" s="73"/>
+      <c r="F9" s="81"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
       <c r="O9" s="74"/>
       <c r="P9" s="74" t="s">
         <v>27</v>
@@ -7898,43 +7885,43 @@
       <c r="Q9" s="74"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A10" s="78"/>
-      <c r="B10" s="78"/>
-      <c r="C10" s="79"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="5"/>
       <c r="E10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="80"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
-      <c r="N10" s="73"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
       <c r="O10" s="74"/>
       <c r="P10" s="74"/>
       <c r="Q10" s="74"/>
     </row>
     <row r="11" spans="1:17" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="78"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="79"/>
+      <c r="A11" s="79"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="6"/>
       <c r="E11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="80"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="77"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
-      <c r="M11" s="73"/>
-      <c r="N11" s="73"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="76"/>
       <c r="O11" s="74"/>
       <c r="P11" s="74"/>
       <c r="Q11" s="74"/>
@@ -9986,24 +9973,24 @@
       <c r="H7" s="36"/>
       <c r="I7" s="36"/>
       <c r="J7" s="36"/>
-      <c r="K7" s="82" t="s">
+      <c r="K7" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="82"/>
-      <c r="M7" s="82"/>
-      <c r="N7" s="82"/>
-      <c r="O7" s="82"/>
-      <c r="P7" s="82"/>
-      <c r="Q7" s="82"/>
+      <c r="L7" s="83"/>
+      <c r="M7" s="83"/>
+      <c r="N7" s="83"/>
+      <c r="O7" s="83"/>
+      <c r="P7" s="83"/>
+      <c r="Q7" s="83"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A8" s="83" t="s">
+      <c r="A8" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="83" t="s">
+      <c r="B8" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="84" t="s">
+      <c r="C8" s="85" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="38" t="s">
@@ -10012,109 +9999,109 @@
       <c r="E8" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="85" t="s">
+      <c r="F8" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="83" t="s">
+      <c r="G8" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="86" t="s">
+      <c r="H8" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="87" t="s">
+      <c r="I8" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="86" t="s">
+      <c r="J8" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="86" t="s">
+      <c r="K8" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="86" t="s">
+      <c r="L8" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="86" t="s">
+      <c r="M8" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="86" t="s">
+      <c r="N8" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="81" t="s">
+      <c r="O8" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="81" t="s">
+      <c r="P8" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="81" t="s">
+      <c r="Q8" s="82" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A9" s="83"/>
-      <c r="B9" s="83"/>
-      <c r="C9" s="84"/>
+      <c r="A9" s="84"/>
+      <c r="B9" s="84"/>
+      <c r="C9" s="85"/>
       <c r="D9" s="40" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="85"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="88"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="86"/>
-      <c r="M9" s="86"/>
-      <c r="N9" s="86"/>
-      <c r="O9" s="81"/>
-      <c r="P9" s="81" t="s">
+      <c r="F9" s="86"/>
+      <c r="G9" s="84"/>
+      <c r="H9" s="87"/>
+      <c r="I9" s="89"/>
+      <c r="J9" s="87"/>
+      <c r="K9" s="87"/>
+      <c r="L9" s="87"/>
+      <c r="M9" s="87"/>
+      <c r="N9" s="87"/>
+      <c r="O9" s="82"/>
+      <c r="P9" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="Q9" s="81"/>
+      <c r="Q9" s="82"/>
     </row>
     <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="83"/>
-      <c r="B10" s="83"/>
-      <c r="C10" s="84"/>
+      <c r="A10" s="84"/>
+      <c r="B10" s="84"/>
+      <c r="C10" s="85"/>
       <c r="D10" s="42"/>
       <c r="E10" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="85"/>
-      <c r="G10" s="83"/>
-      <c r="H10" s="86"/>
-      <c r="I10" s="88"/>
-      <c r="J10" s="86"/>
-      <c r="K10" s="86"/>
-      <c r="L10" s="86"/>
-      <c r="M10" s="86"/>
-      <c r="N10" s="86"/>
-      <c r="O10" s="81"/>
-      <c r="P10" s="81"/>
-      <c r="Q10" s="81"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="84"/>
+      <c r="H10" s="87"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="87"/>
+      <c r="K10" s="87"/>
+      <c r="L10" s="87"/>
+      <c r="M10" s="87"/>
+      <c r="N10" s="87"/>
+      <c r="O10" s="82"/>
+      <c r="P10" s="82"/>
+      <c r="Q10" s="82"/>
     </row>
     <row r="11" spans="1:17" ht="38.65" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="83"/>
-      <c r="B11" s="83"/>
-      <c r="C11" s="84"/>
+      <c r="A11" s="84"/>
+      <c r="B11" s="84"/>
+      <c r="C11" s="85"/>
       <c r="D11" s="44"/>
       <c r="E11" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="85"/>
-      <c r="G11" s="83"/>
-      <c r="H11" s="86"/>
-      <c r="I11" s="82"/>
-      <c r="J11" s="86"/>
-      <c r="K11" s="86"/>
-      <c r="L11" s="86"/>
-      <c r="M11" s="86"/>
-      <c r="N11" s="86"/>
-      <c r="O11" s="81"/>
-      <c r="P11" s="81"/>
-      <c r="Q11" s="81"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="84"/>
+      <c r="H11" s="87"/>
+      <c r="I11" s="83"/>
+      <c r="J11" s="87"/>
+      <c r="K11" s="87"/>
+      <c r="L11" s="87"/>
+      <c r="M11" s="87"/>
+      <c r="N11" s="87"/>
+      <c r="O11" s="82"/>
+      <c r="P11" s="82"/>
+      <c r="Q11" s="82"/>
     </row>
     <row r="12" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B12" s="46" t="s">
@@ -12391,24 +12378,24 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
-      <c r="K7" s="77" t="s">
+      <c r="K7" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="77"/>
-      <c r="M7" s="77"/>
-      <c r="N7" s="77"/>
-      <c r="O7" s="77"/>
-      <c r="P7" s="77"/>
-      <c r="Q7" s="77"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
+      <c r="Q7" s="75"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -12417,31 +12404,31 @@
       <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="80" t="s">
+      <c r="F8" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="78" t="s">
+      <c r="G8" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="73" t="s">
+      <c r="H8" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="75" t="s">
+      <c r="I8" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="73" t="s">
+      <c r="J8" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="73" t="s">
+      <c r="K8" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="73" t="s">
+      <c r="L8" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="73" t="s">
+      <c r="M8" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="73" t="s">
+      <c r="N8" s="76" t="s">
         <v>21</v>
       </c>
       <c r="O8" s="74" t="s">
@@ -12455,24 +12442,24 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A9" s="78"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="79"/>
+      <c r="A9" s="79"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="80"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="73"/>
-      <c r="M9" s="73"/>
-      <c r="N9" s="73"/>
+      <c r="F9" s="81"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
       <c r="O9" s="74"/>
       <c r="P9" s="74" t="s">
         <v>27</v>
@@ -12480,43 +12467,43 @@
       <c r="Q9" s="74"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A10" s="78"/>
-      <c r="B10" s="78"/>
-      <c r="C10" s="79"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="5"/>
       <c r="E10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="80"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
-      <c r="N10" s="73"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
       <c r="O10" s="74"/>
       <c r="P10" s="74"/>
       <c r="Q10" s="74"/>
     </row>
     <row r="11" spans="1:17" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="78"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="79"/>
+      <c r="A11" s="79"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="6"/>
       <c r="E11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="80"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="77"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
-      <c r="M11" s="73"/>
-      <c r="N11" s="73"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="76"/>
       <c r="O11" s="74"/>
       <c r="P11" s="74"/>
       <c r="Q11" s="74"/>
@@ -13956,24 +13943,24 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
-      <c r="K7" s="77" t="s">
+      <c r="K7" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="77"/>
-      <c r="M7" s="77"/>
-      <c r="N7" s="77"/>
-      <c r="O7" s="77"/>
-      <c r="P7" s="77"/>
-      <c r="Q7" s="77"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
+      <c r="Q7" s="75"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -13982,31 +13969,31 @@
       <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="80" t="s">
+      <c r="F8" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="78" t="s">
+      <c r="G8" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="73" t="s">
+      <c r="H8" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="75" t="s">
+      <c r="I8" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="73" t="s">
+      <c r="J8" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="73" t="s">
+      <c r="K8" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="73" t="s">
+      <c r="L8" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="73" t="s">
+      <c r="M8" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="73" t="s">
+      <c r="N8" s="76" t="s">
         <v>21</v>
       </c>
       <c r="O8" s="74" t="s">
@@ -14020,24 +14007,24 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A9" s="78"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="79"/>
+      <c r="A9" s="79"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="80"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="73"/>
-      <c r="M9" s="73"/>
-      <c r="N9" s="73"/>
+      <c r="F9" s="81"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
       <c r="O9" s="74"/>
       <c r="P9" s="74" t="s">
         <v>27</v>
@@ -14045,43 +14032,43 @@
       <c r="Q9" s="74"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A10" s="78"/>
-      <c r="B10" s="78"/>
-      <c r="C10" s="79"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="5"/>
       <c r="E10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="80"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
-      <c r="N10" s="73"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
       <c r="O10" s="74"/>
       <c r="P10" s="74"/>
       <c r="Q10" s="74"/>
     </row>
     <row r="11" spans="1:17" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="78"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="79"/>
+      <c r="A11" s="79"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="6"/>
       <c r="E11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="80"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="77"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
-      <c r="M11" s="73"/>
-      <c r="N11" s="73"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="76"/>
       <c r="O11" s="74"/>
       <c r="P11" s="74"/>
       <c r="Q11" s="74"/>
@@ -14255,24 +14242,24 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
-      <c r="K7" s="77" t="s">
+      <c r="K7" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="77"/>
-      <c r="M7" s="77"/>
-      <c r="N7" s="77"/>
-      <c r="O7" s="77"/>
-      <c r="P7" s="77"/>
-      <c r="Q7" s="77"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
+      <c r="Q7" s="75"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -14281,31 +14268,31 @@
       <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="80" t="s">
+      <c r="F8" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="78" t="s">
+      <c r="G8" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="73" t="s">
+      <c r="H8" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="75" t="s">
+      <c r="I8" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="73" t="s">
+      <c r="J8" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="73" t="s">
+      <c r="K8" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="73" t="s">
+      <c r="L8" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="73" t="s">
+      <c r="M8" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="73" t="s">
+      <c r="N8" s="76" t="s">
         <v>21</v>
       </c>
       <c r="O8" s="74" t="s">
@@ -14319,24 +14306,24 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A9" s="78"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="79"/>
+      <c r="A9" s="79"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="80"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="73"/>
-      <c r="M9" s="73"/>
-      <c r="N9" s="73"/>
+      <c r="F9" s="81"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
       <c r="O9" s="74"/>
       <c r="P9" s="74" t="s">
         <v>27</v>
@@ -14344,43 +14331,43 @@
       <c r="Q9" s="74"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A10" s="78"/>
-      <c r="B10" s="78"/>
-      <c r="C10" s="79"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="5"/>
       <c r="E10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="80"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
-      <c r="N10" s="73"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
       <c r="O10" s="74"/>
       <c r="P10" s="74"/>
       <c r="Q10" s="74"/>
     </row>
     <row r="11" spans="1:17" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="78"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="79"/>
+      <c r="A11" s="79"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="6"/>
       <c r="E11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="80"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="77"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
-      <c r="M11" s="73"/>
-      <c r="N11" s="73"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="76"/>
       <c r="O11" s="74"/>
       <c r="P11" s="74"/>
       <c r="Q11" s="74"/>
@@ -14505,24 +14492,24 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
-      <c r="K7" s="77" t="s">
+      <c r="K7" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="77"/>
-      <c r="M7" s="77"/>
-      <c r="N7" s="77"/>
-      <c r="O7" s="77"/>
-      <c r="P7" s="77"/>
-      <c r="Q7" s="77"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
+      <c r="Q7" s="75"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -14531,31 +14518,31 @@
       <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="80" t="s">
+      <c r="F8" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="78" t="s">
+      <c r="G8" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="73" t="s">
+      <c r="H8" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="75" t="s">
+      <c r="I8" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="73" t="s">
+      <c r="J8" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="73" t="s">
+      <c r="K8" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="73" t="s">
+      <c r="L8" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="73" t="s">
+      <c r="M8" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="73" t="s">
+      <c r="N8" s="76" t="s">
         <v>21</v>
       </c>
       <c r="O8" s="74" t="s">
@@ -14569,24 +14556,24 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A9" s="78"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="79"/>
+      <c r="A9" s="79"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="80"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="73"/>
-      <c r="M9" s="73"/>
-      <c r="N9" s="73"/>
+      <c r="F9" s="81"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
       <c r="O9" s="74"/>
       <c r="P9" s="74" t="s">
         <v>27</v>
@@ -14594,43 +14581,43 @@
       <c r="Q9" s="74"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A10" s="78"/>
-      <c r="B10" s="78"/>
-      <c r="C10" s="79"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="5"/>
       <c r="E10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="80"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
-      <c r="N10" s="73"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
       <c r="O10" s="74"/>
       <c r="P10" s="74"/>
       <c r="Q10" s="74"/>
     </row>
     <row r="11" spans="1:17" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="78"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="79"/>
+      <c r="A11" s="79"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="6"/>
       <c r="E11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="80"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="77"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
-      <c r="M11" s="73"/>
-      <c r="N11" s="73"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="76"/>
       <c r="O11" s="74"/>
       <c r="P11" s="74"/>
       <c r="Q11" s="74"/>
@@ -14755,24 +14742,24 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
-      <c r="K7" s="77" t="s">
+      <c r="K7" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="77"/>
-      <c r="M7" s="77"/>
-      <c r="N7" s="77"/>
-      <c r="O7" s="77"/>
-      <c r="P7" s="77"/>
-      <c r="Q7" s="77"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
+      <c r="Q7" s="75"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -14781,31 +14768,31 @@
       <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="80" t="s">
+      <c r="F8" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="78" t="s">
+      <c r="G8" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="73" t="s">
+      <c r="H8" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="75" t="s">
+      <c r="I8" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="73" t="s">
+      <c r="J8" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="73" t="s">
+      <c r="K8" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="73" t="s">
+      <c r="L8" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="73" t="s">
+      <c r="M8" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="73" t="s">
+      <c r="N8" s="76" t="s">
         <v>21</v>
       </c>
       <c r="O8" s="74" t="s">
@@ -14819,24 +14806,24 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A9" s="78"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="79"/>
+      <c r="A9" s="79"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="80"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="73"/>
-      <c r="M9" s="73"/>
-      <c r="N9" s="73"/>
+      <c r="F9" s="81"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
       <c r="O9" s="74"/>
       <c r="P9" s="74" t="s">
         <v>27</v>
@@ -14844,43 +14831,43 @@
       <c r="Q9" s="74"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A10" s="78"/>
-      <c r="B10" s="78"/>
-      <c r="C10" s="79"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="5"/>
       <c r="E10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="80"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
-      <c r="N10" s="73"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
       <c r="O10" s="74"/>
       <c r="P10" s="74"/>
       <c r="Q10" s="74"/>
     </row>
     <row r="11" spans="1:17" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="78"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="79"/>
+      <c r="A11" s="79"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="6"/>
       <c r="E11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="80"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="77"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
-      <c r="M11" s="73"/>
-      <c r="N11" s="73"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="76"/>
       <c r="O11" s="74"/>
       <c r="P11" s="74"/>
       <c r="Q11" s="74"/>
@@ -14931,15 +14918,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B65BACC764DA63458896B8B483894278" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7557a2c63f95b561b50b2878390af8b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6d31159e-acee-463f-b982-d8404a695cd9" xmlns:ns3="5cb10dfb-6994-4939-a684-a8afac073853" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d2d6f1944dceae87c51bc805fe6d77c1" ns2:_="" ns3:_="">
     <xsd:import namespace="6d31159e-acee-463f-b982-d8404a695cd9"/>
@@ -15130,6 +15108,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -15142,14 +15129,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{238E1B12-F9AE-473C-9D3A-C66B2E1D37A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7667079-9A68-4BB8-A3C6-C75E333C063A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15164,6 +15143,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{238E1B12-F9AE-473C-9D3A-C66B2E1D37A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added mapping of service levels between TM and OJP (#404)
</commit_message>
<xml_diff>
--- a/docs/transmodel_ojp_mapping/Mapping_OJP_TRANSMODEL_V3.0.xlsx
+++ b/docs/transmodel_ojp_mapping/Mapping_OJP_TRANSMODEL_V3.0.xlsx
@@ -1,28 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ue71603\MG_Daten\github\OJP4\docs\transmodel_ojp_mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C701F349-60FC-4ECE-B7BB-4D105B3E28FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA58C3F1-8757-435B-8C0D-576DBDB3AE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-54285" yWindow="9090" windowWidth="21600" windowHeight="12495" tabRatio="469" activeTab="2" xr2:uid="{92A06D46-43C6-42FE-B5E0-5A99A190FF7F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" tabRatio="469" xr2:uid="{92A06D46-43C6-42FE-B5E0-5A99A190FF7F}"/>
   </bookViews>
   <sheets>
-    <sheet name="OJPTrip" sheetId="1" r:id="rId1"/>
-    <sheet name="OJPPlaceInformation" sheetId="3" r:id="rId2"/>
-    <sheet name="OJPStopEvent" sheetId="2" r:id="rId3"/>
-    <sheet name="OJPExchangePoint" sheetId="4" r:id="rId4"/>
-    <sheet name="OJPMultiPointTrip" sheetId="5" r:id="rId5"/>
-    <sheet name="OJPFare" sheetId="6" r:id="rId6"/>
-    <sheet name="OJPTripInformation" sheetId="7" r:id="rId7"/>
-    <sheet name="OJPAvailability" sheetId="8" r:id="rId8"/>
+    <sheet name="Mapping_Services_QUERY_MODEL" sheetId="9" r:id="rId1"/>
+    <sheet name="OJPTrip" sheetId="1" r:id="rId2"/>
+    <sheet name="OJPPlaceInformation" sheetId="3" r:id="rId3"/>
+    <sheet name="OJPStopEvent" sheetId="2" r:id="rId4"/>
+    <sheet name="OJPExchangePoint" sheetId="4" r:id="rId5"/>
+    <sheet name="OJPMultiPointTrip" sheetId="5" r:id="rId6"/>
+    <sheet name="OJPFare" sheetId="6" r:id="rId7"/>
+    <sheet name="OJPTripInformation" sheetId="7" r:id="rId8"/>
+    <sheet name="OJPAvailability" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2670" uniqueCount="1021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2716" uniqueCount="1048">
   <si>
     <t>column H and I are the important part, H should describe, what happens</t>
   </si>
@@ -3111,6 +3113,88 @@
   </si>
   <si>
     <t>OJPAvailabilityResponse</t>
+  </si>
+  <si>
+    <t>OJP</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>EXCHANGE POINTS REQUST</t>
+  </si>
+  <si>
+    <t>SITUATION REQUEST</t>
+  </si>
+  <si>
+    <t>SERVICE JOURNEY REQUEST</t>
+  </si>
+  <si>
+    <t>STOP FARE REQUEST</t>
+  </si>
+  <si>
+    <t>FARE PRODUCT REQUST</t>
+  </si>
+  <si>
+    <t>TRIP FARE REQUEST</t>
+  </si>
+  <si>
+    <t>OJPTripRequest
+OJPMultipointTripRequest</t>
+  </si>
+  <si>
+    <t>OJPStopEventRequest</t>
+  </si>
+  <si>
+    <t>OJPTripInformationRequest</t>
+  </si>
+  <si>
+    <t>Situations are delivered in the results of other requests (e.g. OJPLocationInformationRequest, OJPStopEventRequest, OJPTripRequest)</t>
+  </si>
+  <si>
+    <t>OJPLocationInformationRequest</t>
+  </si>
+  <si>
+    <t>All within OJPFareRequest</t>
+  </si>
+  <si>
+    <t>Asks for the availability of a VEHICLE, SINGLE JOURNEY</t>
+  </si>
+  <si>
+    <t>OJPExchangePointsRequest</t>
+  </si>
+  <si>
+    <t>OJPStatusRequest</t>
+  </si>
+  <si>
+    <t>Informs about the trip planner</t>
+  </si>
+  <si>
+    <t>OJPTripChangeRequest</t>
+  </si>
+  <si>
+    <t>OJPTripRefineRequest</t>
+  </si>
+  <si>
+    <t>Allows to update a TRIP REQUEST from an already made TRIP RESULT</t>
+  </si>
+  <si>
+    <t>Adds more details to given TRIP RESULTS</t>
+  </si>
+  <si>
+    <t>Mapping of the abstract Transmodel services to OJP</t>
+  </si>
+  <si>
+    <t>Transmodel</t>
+  </si>
+  <si>
+    <t>(SCHEDULE REQUEST)</t>
+  </si>
+  <si>
+    <t>(OJPLineInformationRequest)</t>
+  </si>
+  <si>
+    <t>With OJPLineInformationRequest some information about a LINE is provided. This is a part of SCHEDULE REQUEST.</t>
   </si>
 </sst>
 </file>
@@ -3404,7 +3488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3616,6 +3700,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4175,11 +4260,202 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AAB1CDC-A2F2-4A06-BB2E-638A1C365426}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="23.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.86328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="73" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="12" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E8571E6-8D43-44CC-B9D0-687AC8D4191F}">
   <dimension ref="A1:Q208"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="11" topLeftCell="G90" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="11" topLeftCell="G54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="M106" sqref="A1:XFD1048576"/>
@@ -4249,24 +4525,24 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
-      <c r="K7" s="74" t="s">
+      <c r="K7" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="74"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
+      <c r="Q7" s="75"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -4275,109 +4551,109 @@
       <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="80" t="s">
+      <c r="F8" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="78" t="s">
+      <c r="G8" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="76" t="s">
+      <c r="I8" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="75" t="s">
+      <c r="J8" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="75" t="s">
+      <c r="K8" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="75" t="s">
+      <c r="L8" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="75" t="s">
+      <c r="M8" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="75" t="s">
+      <c r="N8" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="73" t="s">
+      <c r="O8" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="73" t="s">
+      <c r="P8" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="73" t="s">
+      <c r="Q8" s="74" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A9" s="78"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="79"/>
+      <c r="A9" s="79"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="80"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="73"/>
-      <c r="P9" s="73" t="s">
+      <c r="F9" s="81"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="Q9" s="73"/>
+      <c r="Q9" s="74"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A10" s="78"/>
-      <c r="B10" s="78"/>
-      <c r="C10" s="79"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="5"/>
       <c r="E10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="80"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="75"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="75"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="73"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
     </row>
     <row r="11" spans="1:17" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="78"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="79"/>
+      <c r="A11" s="79"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="6"/>
       <c r="E11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="80"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="75"/>
-      <c r="N11" s="75"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="73"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="76"/>
+      <c r="O11" s="74"/>
+      <c r="P11" s="74"/>
+      <c r="Q11" s="74"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B12" s="1" t="s">
@@ -7445,7 +7721,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67F5C9FB-EB55-4D3D-AE2C-4A2AE611540E}">
   <dimension ref="A1:Q137"/>
   <sheetViews>
@@ -7520,24 +7796,24 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
-      <c r="K7" s="74" t="s">
+      <c r="K7" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="74"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
+      <c r="Q7" s="75"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -7546,109 +7822,109 @@
       <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="80" t="s">
+      <c r="F8" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="78" t="s">
+      <c r="G8" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="76" t="s">
+      <c r="I8" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="75" t="s">
+      <c r="J8" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="75" t="s">
+      <c r="K8" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="75" t="s">
+      <c r="L8" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="75" t="s">
+      <c r="M8" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="75" t="s">
+      <c r="N8" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="73" t="s">
+      <c r="O8" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="73" t="s">
+      <c r="P8" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="73" t="s">
+      <c r="Q8" s="74" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A9" s="78"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="79"/>
+      <c r="A9" s="79"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="80"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="73"/>
-      <c r="P9" s="73" t="s">
+      <c r="F9" s="81"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="Q9" s="73"/>
+      <c r="Q9" s="74"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A10" s="78"/>
-      <c r="B10" s="78"/>
-      <c r="C10" s="79"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="5"/>
       <c r="E10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="80"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="75"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="75"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="73"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
     </row>
     <row r="11" spans="1:17" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="78"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="79"/>
+      <c r="A11" s="79"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="6"/>
       <c r="E11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="80"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="75"/>
-      <c r="N11" s="75"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="73"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="76"/>
+      <c r="O11" s="74"/>
+      <c r="P11" s="74"/>
+      <c r="Q11" s="74"/>
     </row>
     <row r="12" spans="1:17" ht="57" x14ac:dyDescent="0.45">
       <c r="B12" s="12" t="s">
@@ -9621,11 +9897,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{263B0D09-B6E7-4C7C-ACBE-4F7EEED01E54}">
   <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="11" topLeftCell="I65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -9697,24 +9973,24 @@
       <c r="H7" s="36"/>
       <c r="I7" s="36"/>
       <c r="J7" s="36"/>
-      <c r="K7" s="82" t="s">
+      <c r="K7" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="82"/>
-      <c r="M7" s="82"/>
-      <c r="N7" s="82"/>
-      <c r="O7" s="82"/>
-      <c r="P7" s="82"/>
-      <c r="Q7" s="82"/>
+      <c r="L7" s="83"/>
+      <c r="M7" s="83"/>
+      <c r="N7" s="83"/>
+      <c r="O7" s="83"/>
+      <c r="P7" s="83"/>
+      <c r="Q7" s="83"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A8" s="83" t="s">
+      <c r="A8" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="83" t="s">
+      <c r="B8" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="84" t="s">
+      <c r="C8" s="85" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="38" t="s">
@@ -9723,109 +9999,109 @@
       <c r="E8" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="85" t="s">
+      <c r="F8" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="83" t="s">
+      <c r="G8" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="86" t="s">
+      <c r="H8" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="87" t="s">
+      <c r="I8" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="86" t="s">
+      <c r="J8" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="86" t="s">
+      <c r="K8" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="86" t="s">
+      <c r="L8" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="86" t="s">
+      <c r="M8" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="86" t="s">
+      <c r="N8" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="81" t="s">
+      <c r="O8" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="81" t="s">
+      <c r="P8" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="81" t="s">
+      <c r="Q8" s="82" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A9" s="83"/>
-      <c r="B9" s="83"/>
-      <c r="C9" s="84"/>
+      <c r="A9" s="84"/>
+      <c r="B9" s="84"/>
+      <c r="C9" s="85"/>
       <c r="D9" s="40" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="85"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="88"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="86"/>
-      <c r="M9" s="86"/>
-      <c r="N9" s="86"/>
-      <c r="O9" s="81"/>
-      <c r="P9" s="81" t="s">
+      <c r="F9" s="86"/>
+      <c r="G9" s="84"/>
+      <c r="H9" s="87"/>
+      <c r="I9" s="89"/>
+      <c r="J9" s="87"/>
+      <c r="K9" s="87"/>
+      <c r="L9" s="87"/>
+      <c r="M9" s="87"/>
+      <c r="N9" s="87"/>
+      <c r="O9" s="82"/>
+      <c r="P9" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="Q9" s="81"/>
+      <c r="Q9" s="82"/>
     </row>
     <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="83"/>
-      <c r="B10" s="83"/>
-      <c r="C10" s="84"/>
+      <c r="A10" s="84"/>
+      <c r="B10" s="84"/>
+      <c r="C10" s="85"/>
       <c r="D10" s="42"/>
       <c r="E10" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="85"/>
-      <c r="G10" s="83"/>
-      <c r="H10" s="86"/>
-      <c r="I10" s="88"/>
-      <c r="J10" s="86"/>
-      <c r="K10" s="86"/>
-      <c r="L10" s="86"/>
-      <c r="M10" s="86"/>
-      <c r="N10" s="86"/>
-      <c r="O10" s="81"/>
-      <c r="P10" s="81"/>
-      <c r="Q10" s="81"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="84"/>
+      <c r="H10" s="87"/>
+      <c r="I10" s="89"/>
+      <c r="J10" s="87"/>
+      <c r="K10" s="87"/>
+      <c r="L10" s="87"/>
+      <c r="M10" s="87"/>
+      <c r="N10" s="87"/>
+      <c r="O10" s="82"/>
+      <c r="P10" s="82"/>
+      <c r="Q10" s="82"/>
     </row>
     <row r="11" spans="1:17" ht="38.65" hidden="1" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="83"/>
-      <c r="B11" s="83"/>
-      <c r="C11" s="84"/>
+      <c r="A11" s="84"/>
+      <c r="B11" s="84"/>
+      <c r="C11" s="85"/>
       <c r="D11" s="44"/>
       <c r="E11" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="85"/>
-      <c r="G11" s="83"/>
-      <c r="H11" s="86"/>
-      <c r="I11" s="82"/>
-      <c r="J11" s="86"/>
-      <c r="K11" s="86"/>
-      <c r="L11" s="86"/>
-      <c r="M11" s="86"/>
-      <c r="N11" s="86"/>
-      <c r="O11" s="81"/>
-      <c r="P11" s="81"/>
-      <c r="Q11" s="81"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="84"/>
+      <c r="H11" s="87"/>
+      <c r="I11" s="83"/>
+      <c r="J11" s="87"/>
+      <c r="K11" s="87"/>
+      <c r="L11" s="87"/>
+      <c r="M11" s="87"/>
+      <c r="N11" s="87"/>
+      <c r="O11" s="82"/>
+      <c r="P11" s="82"/>
+      <c r="Q11" s="82"/>
     </row>
     <row r="12" spans="1:17" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B12" s="46" t="s">
@@ -12027,7 +12303,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D88EFA50-F472-477D-861C-0C84615FC860}">
   <dimension ref="A1:Q94"/>
   <sheetViews>
@@ -12102,24 +12378,24 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
-      <c r="K7" s="74" t="s">
+      <c r="K7" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="74"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
+      <c r="Q7" s="75"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -12128,109 +12404,109 @@
       <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="80" t="s">
+      <c r="F8" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="78" t="s">
+      <c r="G8" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="76" t="s">
+      <c r="I8" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="75" t="s">
+      <c r="J8" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="75" t="s">
+      <c r="K8" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="75" t="s">
+      <c r="L8" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="75" t="s">
+      <c r="M8" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="75" t="s">
+      <c r="N8" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="73" t="s">
+      <c r="O8" s="74" t="s">
         <v>898</v>
       </c>
-      <c r="P8" s="73" t="s">
+      <c r="P8" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="73" t="s">
+      <c r="Q8" s="74" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A9" s="78"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="79"/>
+      <c r="A9" s="79"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="80"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="73"/>
-      <c r="P9" s="73" t="s">
+      <c r="F9" s="81"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="Q9" s="73"/>
+      <c r="Q9" s="74"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A10" s="78"/>
-      <c r="B10" s="78"/>
-      <c r="C10" s="79"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="5"/>
       <c r="E10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="80"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="75"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="75"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="73"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
     </row>
     <row r="11" spans="1:17" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="78"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="79"/>
+      <c r="A11" s="79"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="6"/>
       <c r="E11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="80"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="75"/>
-      <c r="N11" s="75"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="73"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="76"/>
+      <c r="O11" s="74"/>
+      <c r="P11" s="74"/>
+      <c r="Q11" s="74"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B12" s="12" t="s">
@@ -13592,7 +13868,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E226BA5-A209-4D27-B7B0-834B796D9DCE}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
@@ -13667,24 +13943,24 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
-      <c r="K7" s="74" t="s">
+      <c r="K7" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="74"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
+      <c r="Q7" s="75"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -13693,109 +13969,109 @@
       <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="80" t="s">
+      <c r="F8" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="78" t="s">
+      <c r="G8" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="76" t="s">
+      <c r="I8" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="75" t="s">
+      <c r="J8" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="75" t="s">
+      <c r="K8" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="75" t="s">
+      <c r="L8" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="75" t="s">
+      <c r="M8" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="75" t="s">
+      <c r="N8" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="73" t="s">
+      <c r="O8" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="73" t="s">
+      <c r="P8" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="73" t="s">
+      <c r="Q8" s="74" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A9" s="78"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="79"/>
+      <c r="A9" s="79"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="80"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="73"/>
-      <c r="P9" s="73" t="s">
+      <c r="F9" s="81"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="Q9" s="73"/>
+      <c r="Q9" s="74"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A10" s="78"/>
-      <c r="B10" s="78"/>
-      <c r="C10" s="79"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="5"/>
       <c r="E10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="80"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="75"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="75"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="73"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
     </row>
     <row r="11" spans="1:17" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="78"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="79"/>
+      <c r="A11" s="79"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="6"/>
       <c r="E11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="80"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="75"/>
-      <c r="N11" s="75"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="73"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="76"/>
+      <c r="O11" s="74"/>
+      <c r="P11" s="74"/>
+      <c r="Q11" s="74"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B12" s="12" t="s">
@@ -13891,7 +14167,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB81E20B-984F-4AFA-941D-66CD7064B644}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
@@ -13966,24 +14242,24 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
-      <c r="K7" s="74" t="s">
+      <c r="K7" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="74"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
+      <c r="Q7" s="75"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -13992,109 +14268,109 @@
       <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="80" t="s">
+      <c r="F8" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="78" t="s">
+      <c r="G8" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="76" t="s">
+      <c r="I8" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="75" t="s">
+      <c r="J8" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="75" t="s">
+      <c r="K8" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="75" t="s">
+      <c r="L8" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="75" t="s">
+      <c r="M8" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="75" t="s">
+      <c r="N8" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="73" t="s">
+      <c r="O8" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="73" t="s">
+      <c r="P8" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="73" t="s">
+      <c r="Q8" s="74" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A9" s="78"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="79"/>
+      <c r="A9" s="79"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="80"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="73"/>
-      <c r="P9" s="73" t="s">
+      <c r="F9" s="81"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="Q9" s="73"/>
+      <c r="Q9" s="74"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A10" s="78"/>
-      <c r="B10" s="78"/>
-      <c r="C10" s="79"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="5"/>
       <c r="E10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="80"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="75"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="75"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="73"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
     </row>
     <row r="11" spans="1:17" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="78"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="79"/>
+      <c r="A11" s="79"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="6"/>
       <c r="E11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="80"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="75"/>
-      <c r="N11" s="75"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="73"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="76"/>
+      <c r="O11" s="74"/>
+      <c r="P11" s="74"/>
+      <c r="Q11" s="74"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B12" s="12" t="s">
@@ -14141,7 +14417,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB730EB-B5B4-4F44-BC03-FF58454E5B15}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
@@ -14216,24 +14492,24 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
-      <c r="K7" s="74" t="s">
+      <c r="K7" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="74"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
+      <c r="Q7" s="75"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -14242,109 +14518,109 @@
       <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="80" t="s">
+      <c r="F8" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="78" t="s">
+      <c r="G8" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="76" t="s">
+      <c r="I8" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="75" t="s">
+      <c r="J8" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="75" t="s">
+      <c r="K8" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="75" t="s">
+      <c r="L8" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="75" t="s">
+      <c r="M8" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="75" t="s">
+      <c r="N8" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="73" t="s">
+      <c r="O8" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="73" t="s">
+      <c r="P8" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="73" t="s">
+      <c r="Q8" s="74" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A9" s="78"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="79"/>
+      <c r="A9" s="79"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="80"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="73"/>
-      <c r="P9" s="73" t="s">
+      <c r="F9" s="81"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="Q9" s="73"/>
+      <c r="Q9" s="74"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A10" s="78"/>
-      <c r="B10" s="78"/>
-      <c r="C10" s="79"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="5"/>
       <c r="E10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="80"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="75"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="75"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="73"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
     </row>
     <row r="11" spans="1:17" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="78"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="79"/>
+      <c r="A11" s="79"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="6"/>
       <c r="E11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="80"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="75"/>
-      <c r="N11" s="75"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="73"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="76"/>
+      <c r="O11" s="74"/>
+      <c r="P11" s="74"/>
+      <c r="Q11" s="74"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B12" s="12" t="s">
@@ -14391,7 +14667,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1A5EACF-ADC6-4FEB-8695-B5A0F0F2CF40}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
@@ -14466,24 +14742,24 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
-      <c r="K7" s="74" t="s">
+      <c r="K7" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="74"/>
+      <c r="L7" s="75"/>
+      <c r="M7" s="75"/>
+      <c r="N7" s="75"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
+      <c r="Q7" s="75"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="78" t="s">
+      <c r="B8" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="80" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -14492,109 +14768,109 @@
       <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="80" t="s">
+      <c r="F8" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="78" t="s">
+      <c r="G8" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="76" t="s">
+      <c r="I8" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="75" t="s">
+      <c r="J8" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="75" t="s">
+      <c r="K8" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="75" t="s">
+      <c r="L8" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="75" t="s">
+      <c r="M8" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="N8" s="75" t="s">
+      <c r="N8" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="O8" s="73" t="s">
+      <c r="O8" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="P8" s="73" t="s">
+      <c r="P8" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="73" t="s">
+      <c r="Q8" s="74" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A9" s="78"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="79"/>
+      <c r="A9" s="79"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="80"/>
       <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="80"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="73"/>
-      <c r="P9" s="73" t="s">
+      <c r="F9" s="81"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="Q9" s="73"/>
+      <c r="Q9" s="74"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A10" s="78"/>
-      <c r="B10" s="78"/>
-      <c r="C10" s="79"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="5"/>
       <c r="E10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="80"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="75"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="75"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="73"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
+      <c r="O10" s="74"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
     </row>
     <row r="11" spans="1:17" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="78"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="79"/>
+      <c r="A11" s="79"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="6"/>
       <c r="E11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="80"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="75"/>
-      <c r="N11" s="75"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="73"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="76"/>
+      <c r="O11" s="74"/>
+      <c r="P11" s="74"/>
+      <c r="Q11" s="74"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="B12" s="12" t="s">
@@ -14642,17 +14918,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="5cb10dfb-6994-4939-a684-a8afac073853" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6d31159e-acee-463f-b982-d8404a695cd9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B65BACC764DA63458896B8B483894278" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7557a2c63f95b561b50b2878390af8b7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6d31159e-acee-463f-b982-d8404a695cd9" xmlns:ns3="5cb10dfb-6994-4939-a684-a8afac073853" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d2d6f1944dceae87c51bc805fe6d77c1" ns2:_="" ns3:_="">
     <xsd:import namespace="6d31159e-acee-463f-b982-d8404a695cd9"/>
@@ -14843,7 +15108,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -14852,24 +15117,18 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{653B82CE-EE8E-41C3-B660-792AB41AF78C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5cb10dfb-6994-4939-a684-a8afac073853"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="6d31159e-acee-463f-b982-d8404a695cd9"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="5cb10dfb-6994-4939-a684-a8afac073853" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6d31159e-acee-463f-b982-d8404a695cd9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7667079-9A68-4BB8-A3C6-C75E333C063A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14888,10 +15147,27 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{238E1B12-F9AE-473C-9D3A-C66B2E1D37A4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{653B82CE-EE8E-41C3-B660-792AB41AF78C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5cb10dfb-6994-4939-a684-a8afac073853"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="6d31159e-acee-463f-b982-d8404a695cd9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>